<commit_message>
Meta updates + code for million cup
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/VellsarMeta.xlsx
+++ b/Excel_and_CSV/VellsarMeta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818F13C1-D2AE-4A77-854A-DE6F73802681}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DF4B76-C03E-42D5-AD19-D4A5A250C352}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="20370" windowHeight="10620" xr2:uid="{7EC583D9-1A7C-40BB-9E54-3D901F246F53}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7EC583D9-1A7C-40BB-9E54-3D901F246F53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="257">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -105,18 +105,6 @@
     <t>Shipsbane Plesiosaurus</t>
   </si>
   <si>
-    <t>Turncoat Dragon Summoner</t>
-  </si>
-  <si>
-    <t>OTK Dragon</t>
-  </si>
-  <si>
-    <t>Disrestan, Ocean Harbinger</t>
-  </si>
-  <si>
-    <t>Gabriel, Heavenly Voice</t>
-  </si>
-  <si>
     <t>Jerva Dragon</t>
   </si>
   <si>
@@ -207,9 +195,6 @@
     <t>Amulet Haven</t>
   </si>
   <si>
-    <t>Selena, Sugarkiss Assassin</t>
-  </si>
-  <si>
     <t>Artifact Portal</t>
   </si>
   <si>
@@ -264,15 +249,6 @@
     <t>6yB-y</t>
   </si>
   <si>
-    <t>7007y</t>
-  </si>
-  <si>
-    <t>77ePy</t>
-  </si>
-  <si>
-    <t>6wgKo</t>
-  </si>
-  <si>
     <t>73nqY</t>
   </si>
   <si>
@@ -330,9 +306,6 @@
     <t>719Nc</t>
   </si>
   <si>
-    <t>74zWI</t>
-  </si>
-  <si>
     <t>6zcK2</t>
   </si>
   <si>
@@ -405,12 +378,6 @@
     <t>Invincible Monster Trio</t>
   </si>
   <si>
-    <t>Niyon, Mystic Musician</t>
-  </si>
-  <si>
-    <t>780qI</t>
-  </si>
-  <si>
     <t>Evolution Shadow</t>
   </si>
   <si>
@@ -474,12 +441,6 @@
     <t>Vincent Rune</t>
   </si>
   <si>
-    <t>Razia, Vengeful Cannonlancer</t>
-  </si>
-  <si>
-    <t>77bzY</t>
-  </si>
-  <si>
     <t>Reggie, Peerless Artisan</t>
   </si>
   <si>
@@ -534,12 +495,6 @@
     <t>7AJJS</t>
   </si>
   <si>
-    <t>Alberta, the Autumnblade</t>
-  </si>
-  <si>
-    <t>76VAc</t>
-  </si>
-  <si>
     <t>Sunbright Elf</t>
   </si>
   <si>
@@ -618,12 +573,6 @@
     <t>Defense Dragon</t>
   </si>
   <si>
-    <t>Drache, Fiery Dragonlord</t>
-  </si>
-  <si>
-    <t>7BSYy</t>
-  </si>
-  <si>
     <t>Beating of the Dragonwings</t>
   </si>
   <si>
@@ -654,12 +603,6 @@
     <t>7CDNy</t>
   </si>
   <si>
-    <t>Pyne, Twisted Justice</t>
-  </si>
-  <si>
-    <t>7CZM2</t>
-  </si>
-  <si>
     <t>Robotic Engineer</t>
   </si>
   <si>
@@ -714,10 +657,145 @@
     <t>Evolution Dragon</t>
   </si>
   <si>
-    <t>Roy, Dragonreaver</t>
-  </si>
-  <si>
-    <t>7BQ6Y</t>
+    <t>Jeno, Fanged Tyrant</t>
+  </si>
+  <si>
+    <t>7AfHY</t>
+  </si>
+  <si>
+    <t>Ramp Dragon</t>
+  </si>
+  <si>
+    <t>Flame Pillar Dragonewt</t>
+  </si>
+  <si>
+    <t>7BNgI</t>
+  </si>
+  <si>
+    <t>OTK Sword</t>
+  </si>
+  <si>
+    <t>Sarissa, Luxflash Spear</t>
+  </si>
+  <si>
+    <t>719NS</t>
+  </si>
+  <si>
+    <t>Lucifer, Fallen Angel</t>
+  </si>
+  <si>
+    <t>72Ico</t>
+  </si>
+  <si>
+    <t>Bunny &amp; Baron, Specter Duo</t>
+  </si>
+  <si>
+    <t>733Ro</t>
+  </si>
+  <si>
+    <t>Saha-Lucifer Sword</t>
+  </si>
+  <si>
+    <t>78nfc</t>
+  </si>
+  <si>
+    <t>Frigg</t>
+  </si>
+  <si>
+    <t>Sarcophagus Wraith</t>
+  </si>
+  <si>
+    <t>6yXzC</t>
+  </si>
+  <si>
+    <t>Honorable Thief</t>
+  </si>
+  <si>
+    <t>6_7-M</t>
+  </si>
+  <si>
+    <t>Ark Daemon</t>
+  </si>
+  <si>
+    <t>Ark-Spider Blood</t>
+  </si>
+  <si>
+    <t>7CAxi</t>
+  </si>
+  <si>
+    <t>Ruinweb Spider</t>
+  </si>
+  <si>
+    <t>6yyq6</t>
+  </si>
+  <si>
+    <t>Aria, Miasma Fairy</t>
+  </si>
+  <si>
+    <t>7AJJI</t>
+  </si>
+  <si>
+    <t>Aggro Forest</t>
+  </si>
+  <si>
+    <t>Rivaylian Bandit</t>
+  </si>
+  <si>
+    <t>72BI2</t>
+  </si>
+  <si>
+    <t>Varmint Hunter</t>
+  </si>
+  <si>
+    <t>72c8y</t>
+  </si>
+  <si>
+    <t>6yAHQ</t>
+  </si>
+  <si>
+    <t>Cursed Furor</t>
+  </si>
+  <si>
+    <t>Burial-Rite Shadow</t>
+  </si>
+  <si>
+    <t>Forlorn Necromancer</t>
+  </si>
+  <si>
+    <t>7Bm4o</t>
+  </si>
+  <si>
+    <t>He Who Once Rocked</t>
+  </si>
+  <si>
+    <t>6yaPS</t>
+  </si>
+  <si>
+    <t>Accel-Loxis Forest</t>
+  </si>
+  <si>
+    <t>OTK Shadow</t>
+  </si>
+  <si>
+    <t>70HDs</t>
+  </si>
+  <si>
+    <t>Soul Box</t>
+  </si>
+  <si>
+    <t>Ceres, Bride of the Night</t>
+  </si>
+  <si>
+    <t>7BqzI</t>
+  </si>
+  <si>
+    <t>Wyrmfire Engineer</t>
+  </si>
+  <si>
+    <t>73iyC</t>
+  </si>
+  <si>
+    <t>Evo-Sanctuary Haven</t>
   </si>
 </sst>
 </file>
@@ -1162,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11DFBF7-9F71-4179-B5F3-8C061A06A61C}">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,19 +1269,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1214,42 +1292,42 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>147</v>
+        <v>248</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>171</v>
+        <v>130</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>172</v>
+        <v>129</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>173</v>
+        <v>119</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>174</v>
+        <v>120</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>7</v>
@@ -1259,23 +1337,23 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>166</v>
+      <c r="A4" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>170</v>
+        <v>157</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>7</v>
@@ -1286,54 +1364,75 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>153</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>11</v>
+        <v>154</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>73</v>
+        <v>155</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>11</v>
+        <v>234</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>131</v>
+        <v>235</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>7</v>
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="C7" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>240</v>
+      </c>
       <c r="G7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1352,13 +1451,13 @@
         <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>7</v>
@@ -1368,169 +1467,179 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="C10" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F10" t="s">
+        <v>164</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="F11" t="s">
+        <v>211</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="F12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="C13" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="C14" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="D13" t="s">
-        <v>179</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="F13" t="s">
-        <v>179</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="D14" t="s">
-        <v>182</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="F14" t="s">
-        <v>182</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>76</v>
+      <c r="C15" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" t="s">
+        <v>167</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F15" t="s">
+        <v>167</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>7</v>
@@ -1541,22 +1650,22 @@
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>185</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>188</v>
+        <v>21</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>189</v>
+        <v>71</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>7</v>
@@ -1566,23 +1675,23 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>193</v>
+      <c r="A17" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>7</v>
@@ -1593,22 +1702,22 @@
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>108</v>
+      <c r="C18" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>7</v>
@@ -1618,23 +1727,23 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>148</v>
+      <c r="A19" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>77</v>
+        <v>176</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>7</v>
@@ -1645,22 +1754,22 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>133</v>
+        <v>22</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>134</v>
+        <v>72</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>135</v>
+        <v>22</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>7</v>
@@ -1671,22 +1780,22 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>159</v>
+        <v>121</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>160</v>
+        <v>122</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>7</v>
@@ -1696,23 +1805,23 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>23</v>
+      <c r="A22" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>26</v>
+        <v>148</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>79</v>
+        <v>148</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>7</v>
@@ -1723,22 +1832,22 @@
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>196</v>
+        <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>197</v>
+        <v>25</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>198</v>
+        <v>73</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>199</v>
+        <v>25</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>200</v>
+        <v>73</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>7</v>
@@ -1749,22 +1858,22 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>33</v>
+        <v>181</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>83</v>
+      <c r="C24" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>183</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>7</v>
@@ -1775,22 +1884,22 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>7</v>
@@ -1801,22 +1910,22 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>229</v>
+        <v>242</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>7</v>
@@ -1827,22 +1936,22 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>7</v>
@@ -1853,22 +1962,22 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>149</v>
+        <v>254</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>150</v>
+        <v>255</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>7</v>
@@ -1879,22 +1988,22 @@
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>7</v>
@@ -1904,153 +2013,153 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>36</v>
+      <c r="A30" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>92</v>
+        <v>31</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>41</v>
+        <v>110</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>114</v>
+      <c r="A32" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>92</v>
+        <v>152</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>146</v>
+        <v>36</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="D33" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>145</v>
+        <v>38</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>145</v>
+        <v>39</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>144</v>
+        <v>81</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>201</v>
+        <v>243</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>202</v>
+        <v>33</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>244</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>203</v>
+        <v>245</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>205</v>
+        <v>247</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>7</v>
@@ -2061,48 +2170,48 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>128</v>
+        <v>249</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>162</v>
+        <v>251</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>163</v>
+        <v>250</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>126</v>
+        <v>252</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>127</v>
+        <v>253</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>125</v>
+        <v>7</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>124</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>92</v>
+        <v>133</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>7</v>
@@ -2112,205 +2221,205 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
-        <v>45</v>
+      <c r="A38" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H38" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
-        <v>48</v>
+      <c r="A39" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H39" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>206</v>
+      <c r="A40" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>7</v>
+        <v>33</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>51</v>
+        <v>114</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H43" s="2" t="s">
+      <c r="F43" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>155</v>
+      <c r="A44" s="4" t="s">
+        <v>189</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>158</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>50</v>
+        <v>159</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>96</v>
+        <v>191</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>7</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>59</v>
+        <v>206</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>60</v>
+        <v>207</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>101</v>
+        <v>208</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>7</v>
@@ -2320,23 +2429,23 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>53</v>
+      <c r="A46" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E46" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>210</v>
+        <v>42</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>7</v>
@@ -2347,22 +2456,22 @@
     </row>
     <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>56</v>
+        <v>230</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>57</v>
+        <v>229</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>99</v>
+        <v>231</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>58</v>
+        <v>232</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>100</v>
+        <v>233</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>7</v>
@@ -2372,101 +2481,101 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>111</v>
+      <c r="A48" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H48" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H49" s="7" t="s">
+      <c r="H48" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H50" s="7" t="s">
+      <c r="A50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>211</v>
+        <v>90</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>216</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>7</v>
@@ -2477,48 +2586,48 @@
     </row>
     <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>7</v>
+        <v>92</v>
+      </c>
+      <c r="G52" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>129</v>
+      <c r="A53" s="10" t="s">
+        <v>256</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>7</v>
@@ -2529,79 +2638,235 @@
     </row>
     <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
-        <v>156</v>
+        <v>101</v>
       </c>
       <c r="B54" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C54" t="s">
-        <v>158</v>
-      </c>
-      <c r="D54" t="s">
-        <v>157</v>
-      </c>
-      <c r="E54" s="8" t="s">
+      <c r="F59" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C60" t="s">
+        <v>145</v>
+      </c>
+      <c r="D60" t="s">
+        <v>144</v>
+      </c>
+      <c r="E60" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F54" t="s">
-        <v>71</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="D55" t="s">
-        <v>214</v>
-      </c>
-      <c r="E55" t="s">
-        <v>222</v>
-      </c>
-      <c r="F55" t="s">
-        <v>216</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C56" t="s">
-        <v>218</v>
-      </c>
-      <c r="D56" t="s">
-        <v>219</v>
-      </c>
-      <c r="E56" t="s">
-        <v>220</v>
-      </c>
-      <c r="F56" t="s">
-        <v>221</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H56" s="2" t="s">
+      <c r="F60" t="s">
+        <v>66</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="D61" t="s">
+        <v>195</v>
+      </c>
+      <c r="E61" t="s">
+        <v>203</v>
+      </c>
+      <c r="F61" t="s">
+        <v>197</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C62" t="s">
+        <v>199</v>
+      </c>
+      <c r="D62" t="s">
+        <v>200</v>
+      </c>
+      <c r="E62" t="s">
+        <v>201</v>
+      </c>
+      <c r="F62" t="s">
+        <v>202</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H62" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bulk miscellaneous Update before RNC - engine openpyxl clear declaration - added comments - Updated Meta Table
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/VellsarMeta.xlsx
+++ b/Excel_and_CSV/VellsarMeta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DF4B76-C03E-42D5-AD19-D4A5A250C352}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF2AC62-E309-4BEB-AB25-5FAD7CA13144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7EC583D9-1A7C-40BB-9E54-3D901F246F53}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{7EC583D9-1A7C-40BB-9E54-3D901F246F53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="251">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -342,15 +342,6 @@
     <t>6Qzmg</t>
   </si>
   <si>
-    <t>Rally Shadow</t>
-  </si>
-  <si>
-    <t>77ygg</t>
-  </si>
-  <si>
-    <t>Undead Parade</t>
-  </si>
-  <si>
     <t>Face Dragon</t>
   </si>
   <si>
@@ -516,12 +507,6 @@
     <t>7Ahjo</t>
   </si>
   <si>
-    <t>Sword-Swinging Bandit</t>
-  </si>
-  <si>
-    <t>76mGC</t>
-  </si>
-  <si>
     <t>Oluon Sword</t>
   </si>
   <si>
@@ -582,18 +567,6 @@
     <t>Last Words Shadow</t>
   </si>
   <si>
-    <t>Chris, Beyond the Patch</t>
-  </si>
-  <si>
-    <t>Kagero, Swordbound Soul</t>
-  </si>
-  <si>
-    <t>7BoX2</t>
-  </si>
-  <si>
-    <t>7BqzS</t>
-  </si>
-  <si>
     <t>Evolution Blood</t>
   </si>
   <si>
@@ -603,12 +576,6 @@
     <t>7CDNy</t>
   </si>
   <si>
-    <t>Robotic Engineer</t>
-  </si>
-  <si>
-    <t>71QTC</t>
-  </si>
-  <si>
     <t>Machina Portal</t>
   </si>
   <si>
@@ -621,21 +588,6 @@
     <t>6zjf6</t>
   </si>
   <si>
-    <t>Resonance Portal</t>
-  </si>
-  <si>
-    <t>Magna Zero</t>
-  </si>
-  <si>
-    <t>7C-Cy</t>
-  </si>
-  <si>
-    <t>Mechanical Designs</t>
-  </si>
-  <si>
-    <t>75FKw</t>
-  </si>
-  <si>
     <t>Bearminator</t>
   </si>
   <si>
@@ -675,27 +627,12 @@
     <t>OTK Sword</t>
   </si>
   <si>
-    <t>Sarissa, Luxflash Spear</t>
-  </si>
-  <si>
-    <t>719NS</t>
-  </si>
-  <si>
-    <t>Lucifer, Fallen Angel</t>
-  </si>
-  <si>
-    <t>72Ico</t>
-  </si>
-  <si>
     <t>Bunny &amp; Baron, Specter Duo</t>
   </si>
   <si>
     <t>733Ro</t>
   </si>
   <si>
-    <t>Saha-Lucifer Sword</t>
-  </si>
-  <si>
     <t>78nfc</t>
   </si>
   <si>
@@ -771,9 +708,6 @@
     <t>6yaPS</t>
   </si>
   <si>
-    <t>Accel-Loxis Forest</t>
-  </si>
-  <si>
     <t>OTK Shadow</t>
   </si>
   <si>
@@ -796,6 +730,54 @@
   </si>
   <si>
     <t>Evo-Sanctuary Haven</t>
+  </si>
+  <si>
+    <t>Absolute Tolerance</t>
+  </si>
+  <si>
+    <t>7C-D6</t>
+  </si>
+  <si>
+    <t>Lunerian Paladin</t>
+  </si>
+  <si>
+    <t>7CWvy</t>
+  </si>
+  <si>
+    <t>Tolerance Portal</t>
+  </si>
+  <si>
+    <t>6zd2w</t>
+  </si>
+  <si>
+    <t>Syntonization</t>
+  </si>
+  <si>
+    <t>Wicked Rebirth</t>
+  </si>
+  <si>
+    <t>7BpFw</t>
+  </si>
+  <si>
+    <t>Nightmare Devourer</t>
+  </si>
+  <si>
+    <t>6yaPc</t>
+  </si>
+  <si>
+    <t>Garven, Iron Dreadnought</t>
+  </si>
+  <si>
+    <t>7Ahk6</t>
+  </si>
+  <si>
+    <t>Banish Haven</t>
+  </si>
+  <si>
+    <t>Priest of the Cudgel</t>
+  </si>
+  <si>
+    <t>60E5y</t>
   </si>
 </sst>
 </file>
@@ -1240,10 +1222,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11DFBF7-9F71-4179-B5F3-8C061A06A61C}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,16 +1274,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>11</v>
@@ -1312,48 +1294,48 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>248</v>
+        <v>133</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>136</v>
+      <c r="A4" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>7</v>
@@ -1364,22 +1346,22 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>153</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>154</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>234</v>
+        <v>11</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>235</v>
+        <v>68</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>7</v>
@@ -1390,230 +1372,230 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>215</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>11</v>
+        <v>216</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>68</v>
+        <v>217</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>11</v>
+        <v>218</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>120</v>
+        <v>219</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>236</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>237</v>
+        <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>238</v>
+        <v>67</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>239</v>
+        <v>9</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>67</v>
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>7</v>
+        <v>70</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>85</v>
+      <c r="C9" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="F9" t="s">
+        <v>247</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="F10" t="s">
+        <v>195</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13" t="s">
+        <v>162</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D14" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="F10" t="s">
-        <v>164</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="F11" t="s">
-        <v>211</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>162</v>
+      <c r="E14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>7</v>
@@ -1623,23 +1605,23 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="F15" t="s">
-        <v>167</v>
+      <c r="E15" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>7</v>
@@ -1649,23 +1631,23 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>19</v>
+      <c r="A16" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>21</v>
+        <v>174</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>71</v>
+        <v>175</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>7</v>
@@ -1675,23 +1657,23 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>174</v>
+      <c r="E17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>7</v>
@@ -1701,23 +1683,23 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>178</v>
+      <c r="A18" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>179</v>
+      <c r="C18" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>179</v>
+        <v>72</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>180</v>
+        <v>72</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>7</v>
@@ -1727,23 +1709,23 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>175</v>
+      <c r="A19" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>177</v>
+        <v>119</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>99</v>
+        <v>121</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>7</v>
@@ -1754,22 +1736,22 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>22</v>
+        <v>144</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>22</v>
+        <v>144</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>7</v>
@@ -1779,23 +1761,23 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>121</v>
+      <c r="A21" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>122</v>
+        <v>24</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>124</v>
+        <v>73</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>125</v>
+        <v>73</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>7</v>
@@ -1805,23 +1787,23 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>146</v>
+      <c r="A22" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>147</v>
+        <v>24</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>147</v>
+        <v>198</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>177</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>7</v>
@@ -1832,22 +1814,22 @@
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>73</v>
+      <c r="C23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>7</v>
@@ -1858,22 +1840,22 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>183</v>
+      <c r="C24" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>7</v>
@@ -1884,22 +1866,22 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>7</v>
@@ -1910,22 +1892,22 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>209</v>
+        <v>105</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>158</v>
+        <v>232</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>159</v>
+        <v>233</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>241</v>
+        <v>135</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>136</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>7</v>
@@ -1936,22 +1918,22 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>77</v>
+        <v>109</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>7</v>
@@ -1962,22 +1944,22 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>108</v>
+        <v>196</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>254</v>
+        <v>31</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>255</v>
+        <v>75</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>139</v>
+        <v>31</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>7</v>
@@ -1988,22 +1970,22 @@
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>7</v>
@@ -2013,153 +1995,153 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>212</v>
+      <c r="A30" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>7</v>
+        <v>149</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>109</v>
+        <v>36</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>110</v>
+        <v>38</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>32</v>
+      <c r="A32" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>84</v>
+        <v>223</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>36</v>
+        <v>227</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>37</v>
+        <v>229</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>79</v>
+        <v>228</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>38</v>
+        <v>230</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>80</v>
+        <v>231</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>243</v>
+        <v>132</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>244</v>
+        <v>40</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>245</v>
+        <v>82</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>246</v>
+        <v>131</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>247</v>
+        <v>130</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>7</v>
@@ -2170,22 +2152,22 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>249</v>
+        <v>179</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>251</v>
+      <c r="C36" s="13" t="s">
+        <v>242</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>252</v>
+        <v>243</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>244</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>7</v>
@@ -2196,48 +2178,48 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>83</v>
+        <v>147</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>134</v>
+        <v>204</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>133</v>
+        <v>205</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>134</v>
+        <v>35</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>133</v>
+        <v>84</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>7</v>
@@ -2247,179 +2229,179 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>184</v>
+      <c r="A39" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>117</v>
+      <c r="A40" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>115</v>
+        <v>42</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>114</v>
+      <c r="A41" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>84</v>
+        <v>42</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>7</v>
+        <v>191</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>7</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
-        <v>41</v>
+      <c r="A42" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H42" s="4" t="s">
+      <c r="C42" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
-        <v>44</v>
+      <c r="A43" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H43" s="4" t="s">
+      <c r="C43" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>189</v>
+      <c r="A44" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>191</v>
+      <c r="C44" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>207</v>
+        <v>7</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>208</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>206</v>
+        <v>123</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>207</v>
+        <v>6</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>208</v>
+        <v>66</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>207</v>
+        <v>124</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>208</v>
+        <v>125</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>7</v>
@@ -2430,22 +2412,22 @@
     </row>
     <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>47</v>
+        <v>139</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>89</v>
+      <c r="C46" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>7</v>
@@ -2456,22 +2438,22 @@
     </row>
     <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>230</v>
+        <v>55</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>229</v>
+        <v>203</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>232</v>
+        <v>188</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>233</v>
+        <v>189</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>7</v>
@@ -2481,23 +2463,23 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>126</v>
+      <c r="A48" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>128</v>
+        <v>50</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>238</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>7</v>
@@ -2508,48 +2490,48 @@
     </row>
     <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G49" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>55</v>
+      <c r="A50" s="10" t="s">
+        <v>234</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>224</v>
+        <v>53</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>205</v>
+        <v>91</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>7</v>
@@ -2559,205 +2541,205 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51" s="2" t="s">
+      <c r="A51" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E51" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>217</v>
+      <c r="C51" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H51" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B52" s="2" t="s">
+      <c r="H51" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E52" s="2" t="s">
+      <c r="C52" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="E53" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F53" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="G52" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="B53" s="2" t="s">
+      <c r="G53" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>103</v>
+      <c r="C54" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>103</v>
+        <v>92</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G54" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G54" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H55" s="7" t="s">
+    <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H56" s="7" t="s">
+      <c r="A56" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B57" s="2" t="s">
+      <c r="A57" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>7</v>
+      <c r="C57" t="s">
+        <v>235</v>
+      </c>
+      <c r="D57" t="s">
+        <v>236</v>
+      </c>
+      <c r="E57" t="s">
+        <v>235</v>
+      </c>
+      <c r="F57" t="s">
+        <v>236</v>
+      </c>
+      <c r="G57" t="s">
+        <v>61</v>
+      </c>
+      <c r="H57" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B58" s="2" t="s">
+      <c r="A58" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>94</v>
+      <c r="C58" t="s">
+        <v>61</v>
+      </c>
+      <c r="D58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E58" t="s">
+        <v>62</v>
+      </c>
+      <c r="F58" t="s">
+        <v>96</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>7</v>
@@ -2767,23 +2749,23 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B59" s="2" t="s">
+      <c r="A59" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>96</v>
+      <c r="C59" t="s">
+        <v>142</v>
+      </c>
+      <c r="D59" t="s">
+        <v>141</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F59" t="s">
+        <v>66</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>7</v>
@@ -2794,79 +2776,27 @@
     </row>
     <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C60" t="s">
-        <v>145</v>
+      <c r="C60" s="14" t="s">
+        <v>185</v>
       </c>
       <c r="D60" t="s">
-        <v>144</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>6</v>
+        <v>184</v>
+      </c>
+      <c r="E60" t="s">
+        <v>187</v>
       </c>
       <c r="F60" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C61" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="D61" t="s">
-        <v>195</v>
-      </c>
-      <c r="E61" t="s">
-        <v>203</v>
-      </c>
-      <c r="F61" t="s">
-        <v>197</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C62" t="s">
-        <v>199</v>
-      </c>
-      <c r="D62" t="s">
-        <v>200</v>
-      </c>
-      <c r="E62" t="s">
-        <v>201</v>
-      </c>
-      <c r="F62" t="s">
-        <v>202</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H62" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>